<commit_message>
Modification on branch C4
</commit_message>
<xml_diff>
--- a/1140310415-Lab1-code/测试样例.xlsx
+++ b/1140310415-Lab1-code/测试样例.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LouYJ\Desktop\Software Engineering\Lab\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Loj/Desktop/Lab1/1140310415-Lab1-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="143">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -520,24 +526,27 @@
   </si>
   <si>
     <t>52</t>
+  </si>
+  <si>
+    <t>//It's on branch C4.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -561,16 +570,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,7 +610,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -879,851 +888,842 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.6640625" style="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="E3" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="E6" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="E7" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="E8" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" s="3">
         <v>41</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="3">
         <v>41</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="E9" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="E11" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="E12" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4" t="s">
+      <c r="E13" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="E15" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="E16" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>12</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="E17" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>13</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="E19" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>14</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="E20" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>15</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="4" t="s">
+      <c r="E22" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="E25" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="E26" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="E29" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="E30" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="E31" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="E32" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="E35" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
       <c r="E36" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="E38" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="4" t="s">
+      <c r="E39" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="E41" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="E42" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-      <c r="B43" s="4" t="s">
+      <c r="E43" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="E45" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="E46" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-      <c r="B47" s="4" t="s">
+      <c r="E47" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="E49" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="E50" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="E52" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="E53" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="2"/>
-      <c r="B54" s="4" t="s">
+      <c r="E54" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="2"/>
+      <c r="B55" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>80</v>
@@ -1735,12 +1735,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>80</v>
@@ -1752,12 +1752,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>80</v>
@@ -1769,72 +1769,72 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="2"/>
-      <c r="B60" s="4" t="s">
+      <c r="E60" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
+      <c r="B61" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="E62" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>83</v>
@@ -1846,12 +1846,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>83</v>
@@ -1863,12 +1863,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>83</v>
@@ -1880,55 +1880,72 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+      <c r="E67" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>117</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B23:D23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modification on branch B1
</commit_message>
<xml_diff>
--- a/1140310415-Lab1-code/测试样例.xlsx
+++ b/1140310415-Lab1-code/测试样例.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LouYJ\Desktop\Software Engineering\Lab\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Loj/Desktop/Lab1/1140310415-Lab1-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="143">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -520,24 +526,27 @@
   </si>
   <si>
     <t>52</t>
+  </si>
+  <si>
+    <t>//It's on brach B1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -561,16 +570,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,7 +610,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -879,851 +888,839 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.6640625" style="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="E3" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="E6" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="E7" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="E8" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" s="3">
         <v>41</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="3">
         <v>41</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="E9" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="E11" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="E12" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4" t="s">
+      <c r="E13" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="E15" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="E16" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>12</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="E17" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>13</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="E19" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>14</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="E20" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>15</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="4" t="s">
+      <c r="E22" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="E25" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="E26" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="E29" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="E30" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="E31" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="E32" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="E35" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
       <c r="E36" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="E38" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="4" t="s">
+      <c r="E39" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="E41" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="E42" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-      <c r="B43" s="4" t="s">
+      <c r="E43" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="E45" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="E46" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-      <c r="B47" s="4" t="s">
+      <c r="E47" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="E49" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="E50" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="E52" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="E53" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="2"/>
-      <c r="B54" s="4" t="s">
+      <c r="E54" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="2"/>
+      <c r="B55" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>80</v>
@@ -1735,12 +1732,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>80</v>
@@ -1752,12 +1749,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>80</v>
@@ -1769,72 +1766,72 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="2"/>
-      <c r="B60" s="4" t="s">
+      <c r="E60" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
+      <c r="B61" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="E62" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>83</v>
@@ -1846,12 +1843,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>83</v>
@@ -1863,12 +1860,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>83</v>
@@ -1880,55 +1877,72 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+      <c r="E67" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>117</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B23:D23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>